<commit_message>
GPLIM-6065 add arquillian test cases
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/externalLibExistingMetadata.xlsx
+++ b/mercury/src/test/resources/testdata/externalLibExistingMetadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="540">
   <si>
     <t>THESE AUTO-GENERATED LISTS MUST NOT BE EDITED.</t>
   </si>
@@ -1631,6 +1631,15 @@
   </si>
   <si>
     <t>47</t>
+  </si>
+  <si>
+    <t>SM-74PZE</t>
+  </si>
+  <si>
+    <t>SM-318RH</t>
+  </si>
+  <si>
+    <t>SM-41HUN</t>
   </si>
 </sst>
 </file>
@@ -1690,8 +1699,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1731,7 +1742,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1747,6 +1758,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1762,6 +1774,7 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2262,10 +2275,7 @@
         <v>527</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>527</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>523</v>
+        <v>537</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>524</v>
@@ -2299,10 +2309,7 @@
       <c r="B3" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>527</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>523</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -2338,10 +2345,7 @@
         <v>527</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>527</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>523</v>
+        <v>539</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>526</v>
@@ -2376,10 +2380,7 @@
         <v>527</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>527</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>523</v>
+        <v>538</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>525</v>

</xml_diff>